<commit_message>
Add user management and config loader modules
Implemented user listing API and refactored user status and password reset endpoints to use RESTful patterns. Added UserRecord model and related logic in backend. Introduced config_loader.py and configuration JSON files for subdivisions and templates. Updated app.py to use new UI entry point.
</commit_message>
<xml_diff>
--- a/backend/data/users.xlsx
+++ b/backend/data/users.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,7 +489,42 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2026-01-19T18:33:15.560676+00:00</t>
+          <t>2026-01-19T19:53:48.523191+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>588b3771-b6bc-4281-a305-69592d89bde2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>naruto@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$2b$12$DCLvK/O1ugMj4kfNsQym6uAa1oaJfryLy5HleUkceALfbWWDE8Y/6</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2026-01-19T19:54:51.060431+00:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2026-01-19T19:55:53.809692+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>